<commit_message>
Add continent column to guns data
</commit_message>
<xml_diff>
--- a/datasets/guns.xlsx
+++ b/datasets/guns.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wahl\Documents\Teaching\Teaching Fall 2017\MAT217D\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>country</t>
   </si>
@@ -33,18 +25,30 @@
     <t>hdi</t>
   </si>
   <si>
+    <t>continent</t>
+  </si>
+  <si>
     <t>Argentina</t>
   </si>
   <si>
+    <t>S. America</t>
+  </si>
+  <si>
     <t>Australia</t>
   </si>
   <si>
     <t>Austria</t>
   </si>
   <si>
+    <t>Europe</t>
+  </si>
+  <si>
     <t>Barbados</t>
   </si>
   <si>
+    <t>N. America</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
@@ -91,6 +95,9 @@
   </si>
   <si>
     <t>Israel</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
   <si>
     <t>Italy</t>
@@ -159,21 +166,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -272,37 +298,40 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -312,85 +341,26 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFBDC0BF"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF3F3F3F"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -400,10 +370,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -580,40 +550,43 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -638,7 +611,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -664,7 +637,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -690,7 +663,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -716,7 +689,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -742,7 +715,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -768,7 +741,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -794,7 +767,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -820,7 +793,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -846,7 +819,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -859,15 +832,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -876,15 +843,15 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -903,7 +870,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +896,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +922,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +948,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,7 +974,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1000,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1026,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1052,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1111,7 +1078,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1137,7 +1104,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1150,15 +1117,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1172,26 +1133,26 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1221,7 +1182,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1247,7 +1208,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1273,7 +1234,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1299,7 +1260,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1325,7 +1286,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1351,7 +1312,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1377,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,7 +1364,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1429,7 +1390,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1442,634 +1403,752 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="8" customWidth="1"/>
-    <col min="5" max="255" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85156" style="1" customWidth="1"/>
+    <col min="6" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="B2" s="6">
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
         <v>5.65</v>
       </c>
-      <c r="C2" s="6">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.79700000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="C2" s="5">
+        <v>10.2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.797</v>
+      </c>
+      <c r="E2" t="s" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="20.1" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8">
         <v>1.05</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>15</v>
       </c>
-      <c r="D3" s="7">
-        <v>0.92900000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="D3" s="8">
+        <v>0.929</v>
+      </c>
+      <c r="E3" t="s" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" ht="20.1" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2.94</v>
+      </c>
+      <c r="C4" s="8">
+        <v>30.4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.885</v>
+      </c>
+      <c r="E4" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="20.1" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>7.8</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.793</v>
+      </c>
+      <c r="E5" t="s" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="20.1" customHeight="1">
+      <c r="A6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2.43</v>
+      </c>
+      <c r="C6" s="8">
+        <v>17.2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.886</v>
+      </c>
+      <c r="E6" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="20.1" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8">
+        <v>4.78</v>
+      </c>
+      <c r="C7" s="8">
+        <v>30.8</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.908</v>
+      </c>
+      <c r="E7" t="s" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" ht="20.1" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="C8" s="8">
+        <v>10.7</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.805</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
-        <v>2.94</v>
-      </c>
-      <c r="C4" s="7">
-        <v>30.4</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.88500000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="9" ht="20.1" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3.01</v>
+      </c>
+      <c r="C9" s="8">
+        <v>21.7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.796</v>
+      </c>
+      <c r="E9" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="20.1" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="C10" s="8">
+        <v>36.4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="E10" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="20.1" customHeight="1">
+      <c r="A11" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1.76</v>
+      </c>
+      <c r="C11" s="8">
+        <v>16.3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.865</v>
+      </c>
+      <c r="E11" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="20.1" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1.45</v>
+      </c>
+      <c r="C12" s="8">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.895</v>
+      </c>
+      <c r="E12" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="20.1" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2.54</v>
+      </c>
+      <c r="C13" s="8">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.835</v>
+      </c>
+      <c r="E13" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" ht="20.1" customHeight="1">
+      <c r="A14" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3.64</v>
+      </c>
+      <c r="C14" s="8">
+        <v>32</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.882</v>
+      </c>
+      <c r="E14" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" ht="20.1" customHeight="1">
+      <c r="A15" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>31.2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.884</v>
+      </c>
+      <c r="E15" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" ht="20.1" customHeight="1">
+      <c r="A16" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1.1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>30.3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.905</v>
+      </c>
+      <c r="E16" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" ht="20.1" customHeight="1">
+      <c r="A17" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="8">
+        <v>22.5</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.861</v>
+      </c>
+      <c r="E17" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" ht="20.1" customHeight="1">
+      <c r="A18" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.8159999999999999</v>
+      </c>
+      <c r="E18" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" ht="20.1" customHeight="1">
+      <c r="A19" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="C19" s="8">
+        <v>30.3</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.898</v>
+      </c>
+      <c r="E19" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" ht="20.1" customHeight="1">
+      <c r="A20" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="C20" s="8">
+        <v>8.6</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.908</v>
+      </c>
+      <c r="E20" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="20.1" customHeight="1">
+      <c r="A21" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1.86</v>
+      </c>
+      <c r="C21" s="8">
+        <v>7.3</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.888</v>
+      </c>
+      <c r="E21" t="s" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" ht="20.1" customHeight="1">
+      <c r="A22" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1.28</v>
+      </c>
+      <c r="C22" s="8">
+        <v>11.9</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.874</v>
+      </c>
+      <c r="E22" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" ht="20.1" customHeight="1">
+      <c r="A23" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.901</v>
+      </c>
+      <c r="E23" t="s" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" ht="20.1" customHeight="1">
+      <c r="A24" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1.43</v>
+      </c>
+      <c r="C24" s="8">
+        <v>19</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.805</v>
+      </c>
+      <c r="E24" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" ht="20.1" customHeight="1">
+      <c r="A25" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1.61</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="E25" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" ht="20.1" customHeight="1">
+      <c r="A26" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1.81</v>
+      </c>
+      <c r="C26" s="8">
+        <v>15.3</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.867</v>
+      </c>
+      <c r="E26" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" ht="20.1" customHeight="1">
+      <c r="A27" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="B27" s="8">
+        <v>2.16</v>
+      </c>
+      <c r="C27" s="8">
+        <v>11.9</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.832</v>
+      </c>
+      <c r="E27" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" ht="20.1" customHeight="1">
+      <c r="A28" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3.9</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="E28" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" ht="20.1" customHeight="1">
+      <c r="A29" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="B29" s="8">
+        <v>2.66</v>
+      </c>
+      <c r="C29" s="8">
+        <v>22.6</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.908</v>
+      </c>
+      <c r="E29" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7">
-        <v>7.8</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0.79300000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="7">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="C6" s="7">
-        <v>17.2</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.88600000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7">
-        <v>4.78</v>
-      </c>
-      <c r="C7" s="7">
-        <v>30.8</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0.06</v>
-      </c>
-      <c r="C8" s="7">
-        <v>10.7</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.80500000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="30" ht="20.1" customHeight="1">
+      <c r="A30" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1.78</v>
+      </c>
+      <c r="C30" s="8">
+        <v>31.3</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0.9429999999999999</v>
+      </c>
+      <c r="E30" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" ht="20.1" customHeight="1">
+      <c r="A31" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="D31" s="8">
+        <v>0.8129999999999999</v>
+      </c>
+      <c r="E31" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" ht="20.1" customHeight="1">
+      <c r="A32" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1.77</v>
+      </c>
+      <c r="C32" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0.8090000000000001</v>
+      </c>
+      <c r="E32" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" ht="20.1" customHeight="1">
+      <c r="A33" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="B33" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="C33" s="8">
+        <v>19.2</v>
+      </c>
+      <c r="D33" s="8">
+        <v>0.831</v>
+      </c>
+      <c r="E33" t="s" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" ht="20.1" customHeight="1">
+      <c r="A34" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="B34" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="8">
+        <v>0.866</v>
+      </c>
+      <c r="E34" t="s" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" ht="20.1" customHeight="1">
+      <c r="A35" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="B35" s="8">
+        <v>1.75</v>
+      </c>
+      <c r="C35" s="8">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0.834</v>
+      </c>
+      <c r="E35" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" ht="20.1" customHeight="1">
+      <c r="A36" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2.44</v>
+      </c>
+      <c r="C36" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0.884</v>
+      </c>
+      <c r="E36" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" ht="20.1" customHeight="1">
+      <c r="A37" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1.1</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0.897</v>
+      </c>
+      <c r="E37" t="s" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" ht="20.1" customHeight="1">
+      <c r="A38" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="B38" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="C38" s="8">
+        <v>10.4</v>
+      </c>
+      <c r="D38" s="8">
+        <v>0.878</v>
+      </c>
+      <c r="E38" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" ht="20.1" customHeight="1">
+      <c r="A39" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1.47</v>
+      </c>
+      <c r="C39" s="8">
+        <v>31.6</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0.904</v>
+      </c>
+      <c r="E39" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" ht="20.1" customHeight="1">
+      <c r="A40" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="B40" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="C40" s="8">
+        <v>45.7</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0.903</v>
+      </c>
+      <c r="E40" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" ht="20.1" customHeight="1">
+      <c r="A41" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="B41" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C41" s="8">
+        <v>6.2</v>
+      </c>
+      <c r="D41" s="8">
+        <v>0.863</v>
+      </c>
+      <c r="E41" t="s" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" ht="20.1" customHeight="1">
+      <c r="A42" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="B42" s="8">
+        <v>9</v>
+      </c>
+      <c r="C42" s="8">
+        <v>88.8</v>
+      </c>
+      <c r="D42" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="E42" t="s" s="9">
         <v>11</v>
-      </c>
-      <c r="B9" s="7">
-        <v>3.01</v>
-      </c>
-      <c r="C9" s="7">
-        <v>21.7</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.79600000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="C10" s="7">
-        <v>36.4</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1.76</v>
-      </c>
-      <c r="C11" s="7">
-        <v>16.3</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1.45</v>
-      </c>
-      <c r="C12" s="7">
-        <v>12</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.89500000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="7">
-        <v>2.54</v>
-      </c>
-      <c r="C13" s="7">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0.83499999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="7">
-        <v>3.64</v>
-      </c>
-      <c r="C14" s="7">
-        <v>32</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.88200000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7">
-        <v>31.2</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0.88400000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C16" s="7">
-        <v>30.3</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.90500000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="C17" s="7">
-        <v>22.5</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.86099999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="7">
-        <v>0.85</v>
-      </c>
-      <c r="C18" s="7">
-        <v>5.5</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0.81599999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="C19" s="7">
-        <v>30.3</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0.89800000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="7">
-        <v>1.03</v>
-      </c>
-      <c r="C20" s="7">
-        <v>8.6</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1.86</v>
-      </c>
-      <c r="C21" s="7">
-        <v>7.3</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0.88800000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1.28</v>
-      </c>
-      <c r="C22" s="7">
-        <v>11.9</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.874</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0.90100000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="7">
-        <v>1.43</v>
-      </c>
-      <c r="C24" s="7">
-        <v>19</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0.80500000000000005</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="7">
-        <v>1.61</v>
-      </c>
-      <c r="C25" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1.81</v>
-      </c>
-      <c r="C26" s="7">
-        <v>15.3</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.86699999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="7">
-        <v>2.16</v>
-      </c>
-      <c r="C27" s="7">
-        <v>11.9</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0.83199999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="7">
-        <v>0.46</v>
-      </c>
-      <c r="C28" s="7">
-        <v>3.9</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="7">
-        <v>2.66</v>
-      </c>
-      <c r="C29" s="7">
-        <v>22.6</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="7">
-        <v>1.78</v>
-      </c>
-      <c r="C30" s="7">
-        <v>31.3</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0.94299999999999995</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="7">
-        <v>0.26</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="D31" s="7">
-        <v>0.81299999999999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1.77</v>
-      </c>
-      <c r="C32" s="7">
-        <v>8.5</v>
-      </c>
-      <c r="D32" s="7">
-        <v>0.80900000000000005</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="7">
-        <v>0.18</v>
-      </c>
-      <c r="C33" s="7">
-        <v>19.2</v>
-      </c>
-      <c r="D33" s="7">
-        <v>0.83099999999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="7">
-        <v>0.24</v>
-      </c>
-      <c r="C34" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D34" s="7">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="7">
-        <v>1.75</v>
-      </c>
-      <c r="C35" s="7">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D35" s="7">
-        <v>0.83399999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="7">
-        <v>2.44</v>
-      </c>
-      <c r="C36" s="7">
-        <v>13.5</v>
-      </c>
-      <c r="D36" s="7">
-        <v>0.88400000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="7">
-        <v>0.13</v>
-      </c>
-      <c r="C37" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D37" s="7">
-        <v>0.89700000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="7">
-        <v>0.63</v>
-      </c>
-      <c r="C38" s="7">
-        <v>10.4</v>
-      </c>
-      <c r="D38" s="7">
-        <v>0.878</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A39" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="7">
-        <v>1.47</v>
-      </c>
-      <c r="C39" s="7">
-        <v>31.6</v>
-      </c>
-      <c r="D39" s="7">
-        <v>0.90400000000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="C40" s="7">
-        <v>45.7</v>
-      </c>
-      <c r="D40" s="7">
-        <v>0.90300000000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="C41" s="7">
-        <v>6.2</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0.86299999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="7">
-        <v>9</v>
-      </c>
-      <c r="C42" s="7">
-        <v>88.8</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0.91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>